<commit_message>
Adaptive Memory Search scheint zu laufen + stuffNotNeededAnyMore gelöscht
</commit_message>
<xml_diff>
--- a/output/Vergleich TabuSearch - LocalSearch 2015-03-10-15-25-42.xlsx
+++ b/output/Vergleich TabuSearch - LocalSearch 2015-03-10-15-25-42.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Vergleich TabuSearch - LocalSea" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1517,7 +1517,7 @@
   <dimension ref="A2:L58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>